<commit_message>
Report and small issue with text
</commit_message>
<xml_diff>
--- a/Design/ChangeTracker.xlsx
+++ b/Design/ChangeTracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhodr\Desktop\MMP\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB58FDE4-00A6-4D1C-9D42-90829637E087}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9AD5D1-1014-4D56-AE45-793A1AF01C89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,7 +148,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,6 +158,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -174,9 +180,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +490,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,12 +619,14 @@
         <v>13</v>
       </c>
       <c r="K7" s="1"/>
+      <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="L8" s="1"/>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">

</xml_diff>